<commit_message>
fix: change UTM termplate term
</commit_message>
<xml_diff>
--- a/utm-tracking-template.xlsx
+++ b/utm-tracking-template.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yezi/Documents/GitHub/半撇私塾课程/对外下载配套文件/FSNM201-Exercise-Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aban/Documents/半撇私塾课程/Share/FSNM201-Exercise-Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1380" windowWidth="25600" windowHeight="13580" tabRatio="500"/>
+    <workbookView xWindow="1940" yWindow="4220" windowWidth="25600" windowHeight="13580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="UMT 批量生成器" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
   <si>
     <t>日期</t>
   </si>
@@ -111,19 +114,15 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>7days-grow-up</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>7days-grow-up</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>yz-CNM12345678</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>yz-CNM12345678</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>profession-guide</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -145,17 +144,20 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -177,22 +179,26 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -545,7 +551,7 @@
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -664,7 +670,7 @@
         <v>6</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>4</v>
@@ -673,7 +679,7 @@
         <v>7</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>4</v>
@@ -686,7 +692,7 @@
       </c>
       <c r="R2" s="6" t="str">
         <f t="shared" ref="R2:R3" si="0">CONCATENATE(B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2)</f>
-        <v>http://mkg201demo.bpteach.com/?utm_source=zhihu.com&amp;utm_medium=referral&amp;utm_campaign=yz-CNM12345678&amp;utm_term=7days-grow-up&amp;utm_content=textlink</v>
+        <v>http://mkg201demo.bpteach.com/?utm_source=zhihu.com&amp;utm_medium=referral&amp;utm_campaign=yz-CNM12345678&amp;utm_term=profession-guide&amp;utm_content=textlink</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -721,7 +727,7 @@
         <v>6</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>4</v>
@@ -730,7 +736,7 @@
         <v>7</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>4</v>
@@ -743,7 +749,7 @@
       </c>
       <c r="R3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>http://mkg201demo.bpteach.com/?utm_source=jianshu.com&amp;utm_medium=referral&amp;utm_campaign=yz-CNM12345678&amp;utm_term=7days-grow-up&amp;utm_content=textlink</v>
+        <v>http://mkg201demo.bpteach.com/?utm_source=jianshu.com&amp;utm_medium=referral&amp;utm_campaign=yz-CNM12345678&amp;utm_term=profession-guide&amp;utm_content=textlink</v>
       </c>
     </row>
   </sheetData>

</xml_diff>